<commit_message>
feat: Update DocumentDownload and Notebook components to validate URLs and display download links; enhance SubjectDetail to pass volumes as props
</commit_message>
<xml_diff>
--- a/public/online-volume.xlsx
+++ b/public/online-volume.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\eason\Document\taiyu-notebookLM-website\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1023F05D-DA5A-4DFA-974B-DF563E9C5D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE2E75E-6508-4057-B62C-093A3BA120EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$141</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
   <si>
     <t>type</t>
   </si>
@@ -452,13 +455,73 @@
   </si>
   <si>
     <t>運動與健康</t>
+  </si>
+  <si>
+    <t>NotebookLM_URL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Download_URL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://notebooklm.google.com/notebook/31d160a1-35bf-415a-ad3a-4c21503be717</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://notebooklm.google.com/notebook/0a7c3390-ddc2-4e45-aca4-b4785eb5c5d0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://notebooklm.google.com/notebook/98f17e03-d08a-4770-941d-20624ce5accb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://notebooklm.google.com/notebook/d1b46c8a-c80e-4a03-910e-af4d9ac69fff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://notebooklm.google.com/notebook/b1d6795d-fc7b-48f8-bca9-b228106437f9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://notebooklm.google.com/notebook/1e1ae2dd-a561-4eab-a34b-c50e00f3e2fe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/17m-4eEeV9sc30ALTwYkFxkEDmq1N6u7W/view?usp=drive_link</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/13hRjhtS5I41pjMrP5xEIh_5Lu3zRPqSq/view?usp=sharing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Ahoqmj_w_j2UlEbe4fbBcs5KNKcuzxg6/view?usp=sharing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/14wTRvEhOkfrMUoWnuapUCa33PjiMwszI/view?usp=sharing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1FiIjlYSmn_ZLbU4u6znVBcDxPvfXThiz/view?usp=sharing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1ODpZaXZKRQcCV7v17sHiubO_VynPgbmk/view?usp=sharing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://notebooklm.google.tw/notebook/0a7c3390-ddc2-4e45-aca4-b4785eb5c5d0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,18 +543,27 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="10"/>
       <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -533,20 +605,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -846,20 +923,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D141"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="69.140625" customWidth="1"/>
+    <col min="6" max="6" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -872,8 +952,14 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -887,7 +973,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -901,7 +987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -915,7 +1001,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -929,7 +1015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -943,7 +1029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -957,7 +1043,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -971,7 +1057,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -985,7 +1071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -999,7 +1085,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1013,7 +1099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1027,7 +1113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1041,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1055,7 +1141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1068,8 +1154,11 @@
       <c r="D15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1083,7 +1172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1097,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1111,7 +1200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1125,7 +1214,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1139,7 +1228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1153,7 +1242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1167,7 +1256,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1181,7 +1270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1195,7 +1284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1209,7 +1298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1223,7 +1312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1237,7 +1326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1251,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1262,7 +1351,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1275,8 +1364,14 @@
       <c r="D30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1289,8 +1384,14 @@
       <c r="D31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1303,8 +1404,14 @@
       <c r="D32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1317,8 +1424,14 @@
       <c r="D33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1331,8 +1444,14 @@
       <c r="D34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1345,8 +1464,14 @@
       <c r="D35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1360,7 +1485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1374,7 +1499,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1388,7 +1513,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1402,7 +1527,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1416,7 +1541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1430,7 +1555,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1444,7 +1569,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1458,7 +1583,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1472,7 +1597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1486,7 +1611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1500,7 +1625,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1514,7 +1639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1528,7 +1653,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1542,7 +1667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2</v>
       </c>
@@ -1556,7 +1681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
@@ -1570,7 +1695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -1584,7 +1709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -1598,7 +1723,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -1612,7 +1737,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2</v>
       </c>
@@ -1626,7 +1751,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2</v>
       </c>
@@ -1640,7 +1765,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -1654,7 +1779,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -1668,7 +1793,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1682,7 +1807,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2</v>
       </c>
@@ -1696,7 +1821,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2</v>
       </c>
@@ -1710,7 +1835,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2</v>
       </c>
@@ -1724,7 +1849,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
@@ -1738,7 +1863,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2</v>
       </c>
@@ -1752,7 +1877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2</v>
       </c>
@@ -1766,7 +1891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2</v>
       </c>
@@ -1780,7 +1905,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2</v>
       </c>
@@ -1794,7 +1919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2</v>
       </c>
@@ -1808,7 +1933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2</v>
       </c>
@@ -1822,7 +1947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2</v>
       </c>
@@ -1836,7 +1961,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2</v>
       </c>
@@ -1850,7 +1975,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2</v>
       </c>
@@ -1864,7 +1989,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2</v>
       </c>
@@ -1878,7 +2003,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>3</v>
       </c>
@@ -1892,7 +2017,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3</v>
       </c>
@@ -1906,7 +2031,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>3</v>
       </c>
@@ -1920,7 +2045,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3</v>
       </c>
@@ -1934,7 +2059,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>3</v>
       </c>
@@ -1948,7 +2073,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>3</v>
       </c>
@@ -1962,7 +2087,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>3</v>
       </c>
@@ -1976,7 +2101,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>3</v>
       </c>
@@ -1990,7 +2115,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>3</v>
       </c>
@@ -2004,7 +2129,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>3</v>
       </c>
@@ -2018,7 +2143,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>3</v>
       </c>
@@ -2032,7 +2157,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>3</v>
       </c>
@@ -2046,7 +2171,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>3</v>
       </c>
@@ -2060,7 +2185,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>3</v>
       </c>
@@ -2074,7 +2199,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2</v>
       </c>
@@ -2088,7 +2213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>3</v>
       </c>
@@ -2098,11 +2223,11 @@
       <c r="C89" t="s">
         <v>91</v>
       </c>
-      <c r="D89" s="4">
+      <c r="D89" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1</v>
       </c>
@@ -2116,7 +2241,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1</v>
       </c>
@@ -2130,7 +2255,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1</v>
       </c>
@@ -2144,7 +2269,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1</v>
       </c>
@@ -2158,7 +2283,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2</v>
       </c>
@@ -2172,7 +2297,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>3</v>
       </c>
@@ -2182,11 +2307,11 @@
       <c r="C95" t="s">
         <v>97</v>
       </c>
-      <c r="D95" s="4">
+      <c r="D95" s="3">
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1</v>
       </c>
@@ -2200,7 +2325,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1</v>
       </c>
@@ -2214,7 +2339,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2</v>
       </c>
@@ -2224,11 +2349,11 @@
       <c r="C98" t="s">
         <v>100</v>
       </c>
-      <c r="D98" s="4">
+      <c r="D98" s="3">
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2</v>
       </c>
@@ -2238,11 +2363,11 @@
       <c r="C99" t="s">
         <v>101</v>
       </c>
-      <c r="D99" s="4">
+      <c r="D99" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>3</v>
       </c>
@@ -2252,11 +2377,11 @@
       <c r="C100" t="s">
         <v>102</v>
       </c>
-      <c r="D100" s="4">
+      <c r="D100" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>3</v>
       </c>
@@ -2266,11 +2391,11 @@
       <c r="C101" t="s">
         <v>103</v>
       </c>
-      <c r="D101" s="4">
+      <c r="D101" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>3</v>
       </c>
@@ -2280,11 +2405,11 @@
       <c r="C102" t="s">
         <v>104</v>
       </c>
-      <c r="D102" s="4">
+      <c r="D102" s="3">
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>3</v>
       </c>
@@ -2298,7 +2423,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2</v>
       </c>
@@ -2308,11 +2433,11 @@
       <c r="C104" t="s">
         <v>106</v>
       </c>
-      <c r="D104" s="4">
+      <c r="D104" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1</v>
       </c>
@@ -2326,7 +2451,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>3</v>
       </c>
@@ -2336,11 +2461,11 @@
       <c r="C106" t="s">
         <v>108</v>
       </c>
-      <c r="D106" s="4">
+      <c r="D106" s="3">
         <v>49</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>3</v>
       </c>
@@ -2350,11 +2475,11 @@
       <c r="C107" t="s">
         <v>109</v>
       </c>
-      <c r="D107" s="4">
+      <c r="D107" s="3">
         <v>50</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>4</v>
       </c>
@@ -2368,7 +2493,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>4</v>
       </c>
@@ -2382,7 +2507,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>3</v>
       </c>
@@ -2396,7 +2521,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>3</v>
       </c>
@@ -2410,7 +2535,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>3</v>
       </c>
@@ -2424,7 +2549,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>3</v>
       </c>
@@ -2438,7 +2563,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>3</v>
       </c>
@@ -2452,7 +2577,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>3</v>
       </c>
@@ -2466,7 +2591,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>3</v>
       </c>
@@ -2480,7 +2605,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>3</v>
       </c>
@@ -2494,7 +2619,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>3</v>
       </c>
@@ -2508,7 +2633,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>3</v>
       </c>
@@ -2522,7 +2647,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>3</v>
       </c>
@@ -2536,7 +2661,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>3</v>
       </c>
@@ -2550,7 +2675,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>3</v>
       </c>
@@ -2564,7 +2689,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>3</v>
       </c>
@@ -2578,7 +2703,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>3</v>
       </c>
@@ -2592,7 +2717,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>3</v>
       </c>
@@ -2606,7 +2731,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>3</v>
       </c>
@@ -2620,7 +2745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>3</v>
       </c>
@@ -2634,7 +2759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>3</v>
       </c>
@@ -2648,7 +2773,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>3</v>
       </c>
@@ -2662,7 +2787,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>3</v>
       </c>
@@ -2676,7 +2801,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>2</v>
       </c>
@@ -2690,7 +2815,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>1</v>
       </c>
@@ -2704,7 +2829,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>1</v>
       </c>
@@ -2718,7 +2843,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>1</v>
       </c>
@@ -2732,7 +2857,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>1</v>
       </c>
@@ -2746,7 +2871,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>1</v>
       </c>
@@ -2760,7 +2885,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>1</v>
       </c>
@@ -2774,7 +2899,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>1</v>
       </c>
@@ -2788,7 +2913,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>1</v>
       </c>
@@ -2802,7 +2927,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>3</v>
       </c>
@@ -2816,7 +2941,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>3</v>
       </c>
@@ -2831,7 +2956,29 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D141" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E30" r:id="rId1" xr:uid="{2708B4B3-F1D0-465C-A428-6AAEA7D44690}"/>
+    <hyperlink ref="E31" r:id="rId2" xr:uid="{0B85B22F-0FE0-46AE-93EC-51C1E91EAEAE}"/>
+    <hyperlink ref="E32" r:id="rId3" xr:uid="{CCF22814-510B-4A72-B461-842029F0AF21}"/>
+    <hyperlink ref="E33" r:id="rId4" xr:uid="{10684E52-7C3F-4754-A993-B032BC5E2A9C}"/>
+    <hyperlink ref="E34" r:id="rId5" xr:uid="{15077AD9-5435-483E-9F69-98FA7E4DDF8A}"/>
+    <hyperlink ref="E35" r:id="rId6" xr:uid="{5000FF53-209F-452B-897A-B5C067712962}"/>
+    <hyperlink ref="F30" r:id="rId7" xr:uid="{75C87892-A596-4EC4-9CDB-E16F95F9815D}"/>
+    <hyperlink ref="F32" r:id="rId8" xr:uid="{D11C745F-B32A-4E47-AF71-3EED2A9ABEA3}"/>
+    <hyperlink ref="F31" r:id="rId9" xr:uid="{5FEFAF59-6404-467F-9147-C655AEA4ADC9}"/>
+    <hyperlink ref="F33" r:id="rId10" xr:uid="{B74D2878-90F8-426B-AAE5-5EE3AE458FEC}"/>
+    <hyperlink ref="F34" r:id="rId11" xr:uid="{0A97E692-1DE7-4890-99D5-C0A05823C8BC}"/>
+    <hyperlink ref="F35" r:id="rId12" xr:uid="{D66E0BEB-B074-446D-847D-0DB4C92FB41B}"/>
+    <hyperlink ref="E15" r:id="rId13" xr:uid="{1A735738-A80E-4496-B09C-B106A0FF3372}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Update responsive styles across components and add phone-first refinements
</commit_message>
<xml_diff>
--- a/public/online-volume.xlsx
+++ b/public/online-volume.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\eason\Document\taiyu-notebookLM-website\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\eason\document\taiyu-notebookLM-website\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE2E75E-6508-4057-B62C-093A3BA120EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626400AA-9F5B-4B0C-8D61-0BABD3B650E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
   <si>
     <t>type</t>
   </si>
@@ -514,6 +514,14 @@
   </si>
   <si>
     <t>https://notebooklm.google.tw/notebook/0a7c3390-ddc2-4e45-aca4-b4785eb5c5d0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://notebooklm.google.com/notebook/ccbf846f-05d4-4d7e-a63b-dddeda2fc80b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/u/3/folders/1KUtX7NU4aeFedb1sTx3sVHmf-97r3fOt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -923,11 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -959,7 +966,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -973,7 +980,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -987,7 +994,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1001,7 +1008,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1015,7 +1022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1029,7 +1036,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1043,7 +1050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1057,7 +1064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1071,7 +1078,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1085,7 +1092,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1099,7 +1106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1113,7 +1120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1127,7 +1134,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1186,7 +1193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1200,7 +1207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1214,7 +1221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1228,7 +1235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1242,7 +1249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1256,7 +1263,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1270,7 +1277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1284,7 +1291,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1298,7 +1305,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1312,7 +1319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1326,7 +1333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1340,7 +1347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1351,7 +1358,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1371,7 +1378,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1391,7 +1398,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1411,7 +1418,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1431,7 +1438,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1451,7 +1458,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1471,7 +1478,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -1485,7 +1492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1499,7 +1506,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -1513,7 +1520,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1527,7 +1534,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -1541,7 +1548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -1555,7 +1562,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -1569,7 +1576,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -1583,7 +1590,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -1597,7 +1604,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1611,7 +1618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1625,7 +1632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1639,7 +1646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -1653,7 +1660,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -1667,7 +1674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2</v>
       </c>
@@ -1681,7 +1688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
@@ -1695,7 +1702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -1709,7 +1716,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -1723,7 +1730,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -1737,7 +1744,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2</v>
       </c>
@@ -1751,7 +1758,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2</v>
       </c>
@@ -1765,7 +1772,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -1779,7 +1786,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -1793,7 +1800,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -1807,7 +1814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2</v>
       </c>
@@ -1821,7 +1828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2</v>
       </c>
@@ -1835,7 +1842,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2</v>
       </c>
@@ -1849,7 +1856,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
@@ -1863,7 +1870,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2</v>
       </c>
@@ -1877,7 +1884,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2</v>
       </c>
@@ -1891,7 +1898,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2</v>
       </c>
@@ -1905,7 +1912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2</v>
       </c>
@@ -1919,7 +1926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2</v>
       </c>
@@ -1933,7 +1940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2</v>
       </c>
@@ -1947,7 +1954,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2</v>
       </c>
@@ -1961,7 +1968,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2</v>
       </c>
@@ -1975,7 +1982,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2</v>
       </c>
@@ -1989,7 +1996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2</v>
       </c>
@@ -2003,7 +2010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>3</v>
       </c>
@@ -2017,7 +2024,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>3</v>
       </c>
@@ -2031,7 +2038,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>3</v>
       </c>
@@ -2045,7 +2052,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>3</v>
       </c>
@@ -2059,7 +2066,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>3</v>
       </c>
@@ -2073,7 +2080,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>3</v>
       </c>
@@ -2087,7 +2094,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>3</v>
       </c>
@@ -2101,7 +2108,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>3</v>
       </c>
@@ -2115,7 +2122,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>3</v>
       </c>
@@ -2129,7 +2136,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>3</v>
       </c>
@@ -2143,7 +2150,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>3</v>
       </c>
@@ -2157,7 +2164,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>3</v>
       </c>
@@ -2171,7 +2178,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>3</v>
       </c>
@@ -2185,7 +2192,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>3</v>
       </c>
@@ -2199,7 +2206,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2</v>
       </c>
@@ -2213,7 +2220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>3</v>
       </c>
@@ -2227,7 +2234,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1</v>
       </c>
@@ -2241,7 +2248,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1</v>
       </c>
@@ -2255,7 +2262,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1</v>
       </c>
@@ -2269,7 +2276,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1</v>
       </c>
@@ -2283,7 +2290,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2</v>
       </c>
@@ -2297,7 +2304,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>3</v>
       </c>
@@ -2311,7 +2318,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1</v>
       </c>
@@ -2325,7 +2332,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1</v>
       </c>
@@ -2339,7 +2346,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2</v>
       </c>
@@ -2353,7 +2360,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2</v>
       </c>
@@ -2367,7 +2374,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>3</v>
       </c>
@@ -2381,7 +2388,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>3</v>
       </c>
@@ -2395,7 +2402,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>3</v>
       </c>
@@ -2409,7 +2416,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>3</v>
       </c>
@@ -2423,7 +2430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2</v>
       </c>
@@ -2437,7 +2444,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1</v>
       </c>
@@ -2451,7 +2458,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>3</v>
       </c>
@@ -2465,7 +2472,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>3</v>
       </c>
@@ -2479,7 +2486,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>4</v>
       </c>
@@ -2493,7 +2500,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>4</v>
       </c>
@@ -2507,7 +2514,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>3</v>
       </c>
@@ -2521,7 +2528,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>3</v>
       </c>
@@ -2535,7 +2542,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>3</v>
       </c>
@@ -2549,7 +2556,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>3</v>
       </c>
@@ -2563,7 +2570,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>3</v>
       </c>
@@ -2577,7 +2584,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>3</v>
       </c>
@@ -2591,7 +2598,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>3</v>
       </c>
@@ -2605,7 +2612,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>3</v>
       </c>
@@ -2619,7 +2626,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>3</v>
       </c>
@@ -2632,8 +2639,14 @@
       <c r="D118" s="1">
         <v>42</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="E118" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F118" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>3</v>
       </c>
@@ -2647,7 +2660,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>3</v>
       </c>
@@ -2661,7 +2674,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>3</v>
       </c>
@@ -2675,7 +2688,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>3</v>
       </c>
@@ -2689,7 +2702,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>3</v>
       </c>
@@ -2703,7 +2716,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>3</v>
       </c>
@@ -2717,7 +2730,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>3</v>
       </c>
@@ -2731,7 +2744,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>3</v>
       </c>
@@ -2745,7 +2758,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>3</v>
       </c>
@@ -2759,7 +2772,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>3</v>
       </c>
@@ -2773,7 +2786,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>3</v>
       </c>
@@ -2787,7 +2800,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>3</v>
       </c>
@@ -2801,7 +2814,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>2</v>
       </c>
@@ -2815,7 +2828,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>1</v>
       </c>
@@ -2829,7 +2842,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>1</v>
       </c>
@@ -2843,7 +2856,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>1</v>
       </c>
@@ -2857,7 +2870,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>1</v>
       </c>
@@ -2871,7 +2884,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>1</v>
       </c>
@@ -2885,7 +2898,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>1</v>
       </c>
@@ -2899,7 +2912,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>1</v>
       </c>
@@ -2913,7 +2926,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>1</v>
       </c>
@@ -2927,7 +2940,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>3</v>
       </c>
@@ -2941,7 +2954,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>3</v>
       </c>
@@ -2956,13 +2969,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D141" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D141" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E30" r:id="rId1" xr:uid="{2708B4B3-F1D0-465C-A428-6AAEA7D44690}"/>
@@ -2978,6 +2985,8 @@
     <hyperlink ref="F34" r:id="rId11" xr:uid="{0A97E692-1DE7-4890-99D5-C0A05823C8BC}"/>
     <hyperlink ref="F35" r:id="rId12" xr:uid="{D66E0BEB-B074-446D-847D-0DB4C92FB41B}"/>
     <hyperlink ref="E15" r:id="rId13" xr:uid="{1A735738-A80E-4496-B09C-B106A0FF3372}"/>
+    <hyperlink ref="E118" r:id="rId14" xr:uid="{7CFF6F8F-61B6-41CF-94EA-DA88D80B1AF8}"/>
+    <hyperlink ref="F118" r:id="rId15" xr:uid="{F5B7AF0C-F296-4C48-B72C-B92329BFE7FD}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Update online volume data in Excel file
</commit_message>
<xml_diff>
--- a/public/online-volume.xlsx
+++ b/public/online-volume.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\eason\document\taiyu-notebookLM-website\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{626400AA-9F5B-4B0C-8D61-0BABD3B650E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C907D77-5B1E-4D4D-8E60-D43E63E6D9F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,7 +521,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://drive.google.com/drive/u/3/folders/1KUtX7NU4aeFedb1sTx3sVHmf-97r3fOt</t>
+    <t>https://drive.google.com/file/d/1NNIUHPBfNFXf0dzZHFoLdrSbi9hq1LtZ/view?usp=sharing</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -943,7 +943,7 @@
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="69.140625" customWidth="1"/>
-    <col min="6" max="6" width="57.140625" customWidth="1"/>
+    <col min="6" max="6" width="89.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">

</xml_diff>